<commit_message>
Works now. My custom i2c driver works
</commit_message>
<xml_diff>
--- a/Pin_planning.xlsx
+++ b/Pin_planning.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="188">
   <si>
     <t xml:space="preserve">XCZU7EVF MPSOC </t>
   </si>
@@ -565,6 +565,24 @@
   </si>
   <si>
     <t>LED3</t>
+  </si>
+  <si>
+    <t>my_i2c_clk</t>
+  </si>
+  <si>
+    <t>my_i2c_sda</t>
+  </si>
+  <si>
+    <t>DAC_A</t>
+  </si>
+  <si>
+    <t>DAC_B</t>
+  </si>
+  <si>
+    <t>DAC_C</t>
+  </si>
+  <si>
+    <t>DAC_D</t>
   </si>
 </sst>
 </file>
@@ -792,7 +810,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -883,6 +901,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1164,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,9 +1200,10 @@
     <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>85</v>
       </c>
@@ -1193,7 +1215,7 @@
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1213,7 +1235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>127</v>
       </c>
@@ -1242,7 +1264,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>128</v>
       </c>
@@ -1271,7 +1293,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>129</v>
       </c>
@@ -1300,7 +1322,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>68</v>
       </c>
@@ -1329,7 +1351,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>130</v>
       </c>
@@ -1356,7 +1378,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>131</v>
       </c>
@@ -1383,7 +1405,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>132</v>
       </c>
@@ -1410,7 +1432,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>133</v>
       </c>
@@ -1437,7 +1459,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>134</v>
       </c>
@@ -1463,8 +1485,20 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>184</v>
+      </c>
+      <c r="S11" t="s">
+        <v>185</v>
+      </c>
+      <c r="T11" t="s">
+        <v>186</v>
+      </c>
+      <c r="U11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>135</v>
       </c>
@@ -1490,8 +1524,28 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <f>1.8/5</f>
+        <v>0.36</v>
+      </c>
+      <c r="R12">
+        <f>P12*1</f>
+        <v>0.36</v>
+      </c>
+      <c r="S12">
+        <f>P12*2</f>
+        <v>0.72</v>
+      </c>
+      <c r="T12">
+        <f>P12*3</f>
+        <v>1.08</v>
+      </c>
+      <c r="U12">
+        <f>P12*4</f>
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>136</v>
       </c>
@@ -1517,8 +1571,24 @@
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <f>ROUNDDOWN((R12/2.5)*2^16,0)</f>
+        <v>9437</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ref="S13:U13" si="0">ROUNDDOWN((S12/2.5)*2^16,0)</f>
+        <v>18874</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>28311</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="0"/>
+        <v>37748</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>137</v>
       </c>
@@ -1544,8 +1614,24 @@
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="R14" s="35" t="str">
+        <f>DEC2HEX(R13)</f>
+        <v>24DD</v>
+      </c>
+      <c r="S14" s="35" t="str">
+        <f t="shared" ref="S14:U14" si="1">DEC2HEX(S13)</f>
+        <v>49BA</v>
+      </c>
+      <c r="T14" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>6E97</v>
+      </c>
+      <c r="U14" s="35" t="str">
+        <f t="shared" si="1"/>
+        <v>9374</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>75</v>
       </c>
@@ -1572,7 +1658,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>78</v>
       </c>
@@ -1892,7 +1978,9 @@
       <c r="F27" s="16">
         <v>10</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -1919,7 +2007,9 @@
       <c r="F28" s="16">
         <v>12</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="1" t="s">
+        <v>183</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -2391,5 +2481,6 @@
     <mergeCell ref="D1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>